<commit_message>
Eliminacio de la columna priority, afegit la distinció per bici, reordenat columnes, resum de les bicis
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:O41"/>
+  <dimension ref="B2:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Prioritari</t>
+          <t>Tipus Bici</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -484,12 +484,12 @@
       </c>
       <c r="L2" s="1" t="inlineStr">
         <is>
+          <t>Temps Total Ruta</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
           <t>Num Entregues</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>Temps Total Ruta</t>
         </is>
       </c>
       <c r="N2" s="1" t="inlineStr">
@@ -512,8 +512,10 @@
           <t>1721101633540 - 01 - NAPOLES - BALMES - 07:40</t>
         </is>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -549,10 +551,10 @@
         <v>24</v>
       </c>
       <c r="L3" t="n">
+        <v>59</v>
+      </c>
+      <c r="M3" t="n">
         <v>5</v>
-      </c>
-      <c r="M3" t="n">
-        <v>59</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -572,8 +574,10 @@
           <t>1721102082040 - 02 - NAPOLES - GOTIC - 07:45</t>
         </is>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -609,10 +613,10 @@
         <v>13</v>
       </c>
       <c r="L4" t="n">
+        <v>41</v>
+      </c>
+      <c r="M4" t="n">
         <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>41</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -632,8 +636,10 @@
           <t>1721102486645 - 03 - NAPOLES - GOTIC - 08:00</t>
         </is>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -669,10 +675,10 @@
         <v>13</v>
       </c>
       <c r="L5" t="n">
+        <v>27</v>
+      </c>
+      <c r="M5" t="n">
         <v>2</v>
-      </c>
-      <c r="M5" t="n">
-        <v>27</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -692,8 +698,10 @@
           <t>1721102462855 - 04 - NAPOLES - GOTIC - 08:00</t>
         </is>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -729,10 +737,10 @@
         <v>19</v>
       </c>
       <c r="L6" t="n">
+        <v>47</v>
+      </c>
+      <c r="M6" t="n">
         <v>4</v>
-      </c>
-      <c r="M6" t="n">
-        <v>47</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -752,8 +760,10 @@
           <t>1721101989601 - 06 - NAPOLES - BARCELONETA - 08:00</t>
         </is>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -789,10 +799,10 @@
         <v>25</v>
       </c>
       <c r="L7" t="n">
+        <v>60</v>
+      </c>
+      <c r="M7" t="n">
         <v>5</v>
-      </c>
-      <c r="M7" t="n">
-        <v>60</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -812,8 +822,10 @@
           <t>1721101715356 - 07 - NAPOLES - DIAGONAL - W - 08:30</t>
         </is>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -849,10 +861,10 @@
         <v>27</v>
       </c>
       <c r="L8" t="n">
+        <v>62</v>
+      </c>
+      <c r="M8" t="n">
         <v>5</v>
-      </c>
-      <c r="M8" t="n">
-        <v>62</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -872,8 +884,10 @@
           <t>1721102423348 - 05 - NAPOLES - URQUINAONA - 08:00</t>
         </is>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -909,10 +923,10 @@
         <v>19</v>
       </c>
       <c r="L9" t="n">
+        <v>47</v>
+      </c>
+      <c r="M9" t="n">
         <v>4</v>
-      </c>
-      <c r="M9" t="n">
-        <v>47</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -932,8 +946,10 @@
           <t>1721102182608 - 08 - NAPOLES - ENRIC GRANADOS - 09:00</t>
         </is>
       </c>
-      <c r="D10" t="b">
-        <v>0</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -969,10 +985,10 @@
         <v>17</v>
       </c>
       <c r="L10" t="n">
+        <v>38</v>
+      </c>
+      <c r="M10" t="n">
         <v>3</v>
-      </c>
-      <c r="M10" t="n">
-        <v>38</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -992,8 +1008,10 @@
           <t>1721099914915 - 09 - NAPOLES - P9 - W - 09:30</t>
         </is>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1029,10 +1047,10 @@
         <v>30</v>
       </c>
       <c r="L11" t="n">
+        <v>65</v>
+      </c>
+      <c r="M11" t="n">
         <v>5</v>
-      </c>
-      <c r="M11" t="n">
-        <v>65</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1052,8 +1070,10 @@
           <t>1721101666656 - 12 - NAPOLES - BALMES - 10:00</t>
         </is>
       </c>
-      <c r="D12" t="b">
-        <v>0</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1089,10 +1109,10 @@
         <v>23</v>
       </c>
       <c r="L12" t="n">
+        <v>51</v>
+      </c>
+      <c r="M12" t="n">
         <v>4</v>
-      </c>
-      <c r="M12" t="n">
-        <v>51</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1112,8 +1132,10 @@
           <t>1721102522098 - 11 - NAPOLES - GOTIC - W - 10:00</t>
         </is>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1149,10 +1171,10 @@
         <v>19</v>
       </c>
       <c r="L13" t="n">
+        <v>47</v>
+      </c>
+      <c r="M13" t="n">
         <v>4</v>
-      </c>
-      <c r="M13" t="n">
-        <v>47</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1172,8 +1194,10 @@
           <t>1721102546874 - 10 - NAPOLES - CATALUÑA - 10:00</t>
         </is>
       </c>
-      <c r="D14" t="b">
-        <v>0</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1209,10 +1233,10 @@
         <v>20</v>
       </c>
       <c r="L14" t="n">
+        <v>48</v>
+      </c>
+      <c r="M14" t="n">
         <v>4</v>
-      </c>
-      <c r="M14" t="n">
-        <v>48</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1232,8 +1256,10 @@
           <t>1721102119136 - 13 - NAPOLES - CATALUÑA - W - 10:30</t>
         </is>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1269,10 +1295,10 @@
         <v>13</v>
       </c>
       <c r="L15" t="n">
+        <v>48</v>
+      </c>
+      <c r="M15" t="n">
         <v>5</v>
-      </c>
-      <c r="M15" t="n">
-        <v>48</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1292,8 +1318,10 @@
           <t>1721101949589 - 14 - NAPOLES - VERDAGUER - 11:00</t>
         </is>
       </c>
-      <c r="D16" t="b">
-        <v>0</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1329,10 +1357,10 @@
         <v>12</v>
       </c>
       <c r="L16" t="n">
+        <v>26</v>
+      </c>
+      <c r="M16" t="n">
         <v>2</v>
-      </c>
-      <c r="M16" t="n">
-        <v>26</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1352,8 +1380,10 @@
           <t>1721102224478 - 16 - NAPOLES - BORN - 11:30</t>
         </is>
       </c>
-      <c r="D17" t="b">
-        <v>0</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1389,10 +1419,10 @@
         <v>20</v>
       </c>
       <c r="L17" t="n">
+        <v>76</v>
+      </c>
+      <c r="M17" t="n">
         <v>8</v>
-      </c>
-      <c r="M17" t="n">
-        <v>76</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1412,8 +1442,10 @@
           <t>1721102651888 - 15 - NAPOLES - GOTIC - 11:30</t>
         </is>
       </c>
-      <c r="D18" t="b">
-        <v>0</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1449,10 +1481,10 @@
         <v>18</v>
       </c>
       <c r="L18" t="n">
+        <v>46</v>
+      </c>
+      <c r="M18" t="n">
         <v>4</v>
-      </c>
-      <c r="M18" t="n">
-        <v>46</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -1472,8 +1504,10 @@
           <t>1721102627472 - 17 - NAPOLES - GOTIC - 12:00</t>
         </is>
       </c>
-      <c r="D19" t="b">
-        <v>0</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1509,10 +1543,10 @@
         <v>19</v>
       </c>
       <c r="L19" t="n">
+        <v>61</v>
+      </c>
+      <c r="M19" t="n">
         <v>6</v>
-      </c>
-      <c r="M19" t="n">
-        <v>61</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1532,8 +1566,10 @@
           <t>1721102268642 - 18 - NAPOLES - PUERTO - 12:00</t>
         </is>
       </c>
-      <c r="D20" t="b">
-        <v>0</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1569,10 +1605,10 @@
         <v>26</v>
       </c>
       <c r="L20" t="n">
+        <v>40</v>
+      </c>
+      <c r="M20" t="n">
         <v>2</v>
-      </c>
-      <c r="M20" t="n">
-        <v>40</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -1592,8 +1628,10 @@
           <t>1721102689216 - 19 - NAPOLES - TARDE - W - 17:00</t>
         </is>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1629,10 +1667,10 @@
         <v>12</v>
       </c>
       <c r="L21" t="n">
+        <v>19</v>
+      </c>
+      <c r="M21" t="n">
         <v>1</v>
-      </c>
-      <c r="M21" t="n">
-        <v>19</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -1652,8 +1690,10 @@
           <t>1721100355845 - 01 - SANTS - NUMANCIA - 07:40</t>
         </is>
       </c>
-      <c r="D22" t="b">
-        <v>0</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1689,10 +1729,10 @@
         <v>16</v>
       </c>
       <c r="L22" t="n">
+        <v>58</v>
+      </c>
+      <c r="M22" t="n">
         <v>6</v>
-      </c>
-      <c r="M22" t="n">
-        <v>58</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -1712,8 +1752,10 @@
           <t>1721100497594 - 02 - SANTS - TARRADELLAS - 08:00</t>
         </is>
       </c>
-      <c r="D23" t="b">
-        <v>0</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1749,10 +1791,10 @@
         <v>16</v>
       </c>
       <c r="L23" t="n">
+        <v>37</v>
+      </c>
+      <c r="M23" t="n">
         <v>3</v>
-      </c>
-      <c r="M23" t="n">
-        <v>37</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -1772,8 +1814,10 @@
           <t>1721100630101 - 04 - SANTS - BERLIN - 08:30</t>
         </is>
       </c>
-      <c r="D24" t="b">
-        <v>0</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1809,10 +1853,10 @@
         <v>16</v>
       </c>
       <c r="L24" t="n">
+        <v>37</v>
+      </c>
+      <c r="M24" t="n">
         <v>3</v>
-      </c>
-      <c r="M24" t="n">
-        <v>37</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -1832,8 +1876,10 @@
           <t>1721101262949 - 03 - SANTS - RAVAL - 08:30</t>
         </is>
       </c>
-      <c r="D25" t="b">
-        <v>0</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1869,10 +1915,10 @@
         <v>17</v>
       </c>
       <c r="L25" t="n">
+        <v>31</v>
+      </c>
+      <c r="M25" t="n">
         <v>2</v>
-      </c>
-      <c r="M25" t="n">
-        <v>31</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -1892,8 +1938,10 @@
           <t>1721100247896 - 05 - SANTS - ROCAFORT - W - 08:45</t>
         </is>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1929,10 +1977,10 @@
         <v>15</v>
       </c>
       <c r="L26" t="n">
+        <v>50</v>
+      </c>
+      <c r="M26" t="n">
         <v>5</v>
-      </c>
-      <c r="M26" t="n">
-        <v>50</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -1952,8 +2000,10 @@
           <t>1721100922012 - 06 - SANTS - SANT RAMON - W - 09:00</t>
         </is>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1989,10 +2039,10 @@
         <v>31</v>
       </c>
       <c r="L27" t="n">
+        <v>66</v>
+      </c>
+      <c r="M27" t="n">
         <v>5</v>
-      </c>
-      <c r="M27" t="n">
-        <v>66</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -2012,8 +2062,10 @@
           <t>1721100178035 - 07 - SANTS - GOTIC - W - 09:20</t>
         </is>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2049,10 +2101,10 @@
         <v>25</v>
       </c>
       <c r="L28" t="n">
+        <v>67</v>
+      </c>
+      <c r="M28" t="n">
         <v>6</v>
-      </c>
-      <c r="M28" t="n">
-        <v>67</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2072,8 +2124,10 @@
           <t>1721101127690 - 08 - SANTS - CLINIC - W - 09:30</t>
         </is>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2109,10 +2163,10 @@
         <v>14</v>
       </c>
       <c r="L29" t="n">
+        <v>35</v>
+      </c>
+      <c r="M29" t="n">
         <v>3</v>
-      </c>
-      <c r="M29" t="n">
-        <v>35</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
@@ -2132,8 +2186,10 @@
           <t>1721100593141 - 09 - SANTS - NUMANCIA - 09:30</t>
         </is>
       </c>
-      <c r="D30" t="b">
-        <v>0</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2169,10 +2225,10 @@
         <v>19</v>
       </c>
       <c r="L30" t="n">
+        <v>54</v>
+      </c>
+      <c r="M30" t="n">
         <v>5</v>
-      </c>
-      <c r="M30" t="n">
-        <v>54</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -2192,8 +2248,10 @@
           <t>1721100704935 - 12 - SANTS - CLINIC - W - 10:00</t>
         </is>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2229,10 +2287,10 @@
         <v>21</v>
       </c>
       <c r="L31" t="n">
+        <v>63</v>
+      </c>
+      <c r="M31" t="n">
         <v>6</v>
-      </c>
-      <c r="M31" t="n">
-        <v>63</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -2252,8 +2310,10 @@
           <t>1721101164491 - 11 - SANTS - SANT ANTONI - W - 10:00</t>
         </is>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2289,10 +2349,10 @@
         <v>19</v>
       </c>
       <c r="L32" t="n">
+        <v>54</v>
+      </c>
+      <c r="M32" t="n">
         <v>5</v>
-      </c>
-      <c r="M32" t="n">
-        <v>54</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -2312,8 +2372,10 @@
           <t>1721101394043 - 10 - S01 - SANTS - SYNLAB - 10:00</t>
         </is>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -2349,10 +2411,10 @@
         <v>84</v>
       </c>
       <c r="L33" t="n">
+        <v>119</v>
+      </c>
+      <c r="M33" t="n">
         <v>5</v>
-      </c>
-      <c r="M33" t="n">
-        <v>119</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
@@ -2372,8 +2434,10 @@
           <t>1721101237043 - 13 - SANTS - GOTIC - 10:30</t>
         </is>
       </c>
-      <c r="D34" t="b">
-        <v>0</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2409,10 +2473,10 @@
         <v>19</v>
       </c>
       <c r="L34" t="n">
+        <v>40</v>
+      </c>
+      <c r="M34" t="n">
         <v>3</v>
-      </c>
-      <c r="M34" t="n">
-        <v>40</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
@@ -2432,8 +2496,10 @@
           <t>1721100447653 - 15 - SANTS - GOTIC - 11:00</t>
         </is>
       </c>
-      <c r="D35" t="b">
-        <v>0</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2469,10 +2535,10 @@
         <v>23</v>
       </c>
       <c r="L35" t="n">
+        <v>51</v>
+      </c>
+      <c r="M35" t="n">
         <v>4</v>
-      </c>
-      <c r="M35" t="n">
-        <v>51</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
@@ -2492,8 +2558,10 @@
           <t>1721101195978 - 14 - SANTS - ENTENÇA - 11:00</t>
         </is>
       </c>
-      <c r="D36" t="b">
-        <v>0</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2529,10 +2597,10 @@
         <v>11</v>
       </c>
       <c r="L36" t="n">
+        <v>32</v>
+      </c>
+      <c r="M36" t="n">
         <v>3</v>
-      </c>
-      <c r="M36" t="n">
-        <v>32</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
@@ -2552,8 +2620,10 @@
           <t>1721101020078 - 16 - SANTS - ARIBAU - W - 12:00</t>
         </is>
       </c>
-      <c r="D37" t="b">
-        <v>1</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2589,10 +2659,10 @@
         <v>20</v>
       </c>
       <c r="L37" t="n">
+        <v>48</v>
+      </c>
+      <c r="M37" t="n">
         <v>4</v>
-      </c>
-      <c r="M37" t="n">
-        <v>48</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
@@ -2612,8 +2682,10 @@
           <t>1721101422578 - 17 - S02 - SANTS - SYNLAB - 13:00</t>
         </is>
       </c>
-      <c r="D38" t="b">
-        <v>0</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2649,10 +2721,10 @@
         <v>68</v>
       </c>
       <c r="L38" t="n">
+        <v>89</v>
+      </c>
+      <c r="M38" t="n">
         <v>3</v>
-      </c>
-      <c r="M38" t="n">
-        <v>89</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
@@ -2672,8 +2744,10 @@
           <t>1721101452774 - 18 - S03 - SANTS - SYNLAB - 16:00</t>
         </is>
       </c>
-      <c r="D39" t="b">
-        <v>0</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2709,10 +2783,10 @@
         <v>88</v>
       </c>
       <c r="L39" t="n">
+        <v>123</v>
+      </c>
+      <c r="M39" t="n">
         <v>5</v>
-      </c>
-      <c r="M39" t="n">
-        <v>123</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -2732,8 +2806,10 @@
           <t>1721101486211 - 19 - S04 - SANTS - SYNLAB - 18:00</t>
         </is>
       </c>
-      <c r="D40" t="b">
-        <v>0</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2769,10 +2845,10 @@
         <v>69</v>
       </c>
       <c r="L40" t="n">
+        <v>90</v>
+      </c>
+      <c r="M40" t="n">
         <v>3</v>
-      </c>
-      <c r="M40" t="n">
-        <v>90</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
@@ -2869,21 +2945,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2897,21 +2973,21 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>J</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="6">
@@ -2925,7 +3001,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2935,7 +3011,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:55</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -2953,7 +3029,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>O</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2963,11 +3039,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>08:55</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="8">
@@ -2981,17 +3057,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -3009,21 +3085,21 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>R</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1.1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="10">
@@ -3037,21 +3113,21 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="11">
@@ -3065,17 +3141,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -3093,21 +3169,21 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="13">
@@ -3121,21 +3197,21 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>10:08</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.7</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="14">
@@ -3207,8 +3283,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24"/>
-    <row r="25"/>
+    <row r="20">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Trikes</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Percentatge Trikes</t>
+        </is>
+      </c>
+      <c r="G21">
+        <f>G20/G18</f>
+        <v/>
+      </c>
+    </row>
     <row r="26"/>
     <row r="27"/>
     <row r="28"/>
@@ -3220,7 +3315,7 @@
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Prioritari</t>
+          <t>Tipus Bici</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
@@ -3260,12 +3355,12 @@
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
+          <t>Temps Total Ruta</t>
+        </is>
+      </c>
+      <c r="M29" s="1" t="inlineStr">
+        <is>
           <t>Num Entregues</t>
-        </is>
-      </c>
-      <c r="M29" s="1" t="inlineStr">
-        <is>
-          <t>Temps Total Ruta</t>
         </is>
       </c>
       <c r="N29" s="1" t="inlineStr">
@@ -3288,8 +3383,10 @@
           <t>1721101633540 - 01 - NAPOLES - BALMES - 07:40</t>
         </is>
       </c>
-      <c r="D30" t="b">
-        <v>0</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -3325,10 +3422,10 @@
         <v>24</v>
       </c>
       <c r="L30" t="n">
+        <v>59</v>
+      </c>
+      <c r="M30" t="n">
         <v>5</v>
-      </c>
-      <c r="M30" t="n">
-        <v>59</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -3348,8 +3445,10 @@
           <t>1721102082040 - 02 - NAPOLES - GOTIC - 07:45</t>
         </is>
       </c>
-      <c r="D31" t="b">
-        <v>0</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3385,10 +3484,10 @@
         <v>13</v>
       </c>
       <c r="L31" t="n">
+        <v>41</v>
+      </c>
+      <c r="M31" t="n">
         <v>4</v>
-      </c>
-      <c r="M31" t="n">
-        <v>41</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -3408,8 +3507,10 @@
           <t>1721102486645 - 03 - NAPOLES - GOTIC - 08:00</t>
         </is>
       </c>
-      <c r="D32" t="b">
-        <v>0</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -3445,10 +3546,10 @@
         <v>13</v>
       </c>
       <c r="L32" t="n">
+        <v>27</v>
+      </c>
+      <c r="M32" t="n">
         <v>2</v>
-      </c>
-      <c r="M32" t="n">
-        <v>27</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -3468,8 +3569,10 @@
           <t>1721102462855 - 04 - NAPOLES - GOTIC - 08:00</t>
         </is>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -3505,10 +3608,10 @@
         <v>19</v>
       </c>
       <c r="L33" t="n">
+        <v>47</v>
+      </c>
+      <c r="M33" t="n">
         <v>4</v>
-      </c>
-      <c r="M33" t="n">
-        <v>47</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
@@ -3528,8 +3631,10 @@
           <t>1721101989601 - 06 - NAPOLES - BARCELONETA - 08:00</t>
         </is>
       </c>
-      <c r="D34" t="b">
-        <v>0</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -3565,10 +3670,10 @@
         <v>25</v>
       </c>
       <c r="L34" t="n">
+        <v>60</v>
+      </c>
+      <c r="M34" t="n">
         <v>5</v>
-      </c>
-      <c r="M34" t="n">
-        <v>60</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
@@ -3588,8 +3693,10 @@
           <t>1721101715356 - 07 - NAPOLES - DIAGONAL - W - 08:30</t>
         </is>
       </c>
-      <c r="D35" t="b">
-        <v>1</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -3625,10 +3732,10 @@
         <v>27</v>
       </c>
       <c r="L35" t="n">
+        <v>62</v>
+      </c>
+      <c r="M35" t="n">
         <v>5</v>
-      </c>
-      <c r="M35" t="n">
-        <v>62</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
@@ -3648,8 +3755,10 @@
           <t>1721102423348 - 05 - NAPOLES - URQUINAONA - 08:00</t>
         </is>
       </c>
-      <c r="D36" t="b">
-        <v>0</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -3685,10 +3794,10 @@
         <v>19</v>
       </c>
       <c r="L36" t="n">
+        <v>47</v>
+      </c>
+      <c r="M36" t="n">
         <v>4</v>
-      </c>
-      <c r="M36" t="n">
-        <v>47</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
@@ -3708,8 +3817,10 @@
           <t>1721102182608 - 08 - NAPOLES - ENRIC GRANADOS - 09:00</t>
         </is>
       </c>
-      <c r="D37" t="b">
-        <v>0</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -3745,10 +3856,10 @@
         <v>17</v>
       </c>
       <c r="L37" t="n">
+        <v>38</v>
+      </c>
+      <c r="M37" t="n">
         <v>3</v>
-      </c>
-      <c r="M37" t="n">
-        <v>38</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
@@ -3768,8 +3879,10 @@
           <t>1721099914915 - 09 - NAPOLES - P9 - W - 09:30</t>
         </is>
       </c>
-      <c r="D38" t="b">
-        <v>1</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -3805,10 +3918,10 @@
         <v>30</v>
       </c>
       <c r="L38" t="n">
+        <v>65</v>
+      </c>
+      <c r="M38" t="n">
         <v>5</v>
-      </c>
-      <c r="M38" t="n">
-        <v>65</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
@@ -3828,8 +3941,10 @@
           <t>1721101666656 - 12 - NAPOLES - BALMES - 10:00</t>
         </is>
       </c>
-      <c r="D39" t="b">
-        <v>0</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -3865,10 +3980,10 @@
         <v>23</v>
       </c>
       <c r="L39" t="n">
+        <v>51</v>
+      </c>
+      <c r="M39" t="n">
         <v>4</v>
-      </c>
-      <c r="M39" t="n">
-        <v>51</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -3888,8 +4003,10 @@
           <t>1721102522098 - 11 - NAPOLES - GOTIC - W - 10:00</t>
         </is>
       </c>
-      <c r="D40" t="b">
-        <v>1</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -3925,10 +4042,10 @@
         <v>19</v>
       </c>
       <c r="L40" t="n">
+        <v>47</v>
+      </c>
+      <c r="M40" t="n">
         <v>4</v>
-      </c>
-      <c r="M40" t="n">
-        <v>47</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
@@ -3948,8 +4065,10 @@
           <t>1721102546874 - 10 - NAPOLES - CATALUÑA - 10:00</t>
         </is>
       </c>
-      <c r="D41" t="b">
-        <v>0</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -3985,10 +4104,10 @@
         <v>20</v>
       </c>
       <c r="L41" t="n">
+        <v>48</v>
+      </c>
+      <c r="M41" t="n">
         <v>4</v>
-      </c>
-      <c r="M41" t="n">
-        <v>48</v>
       </c>
       <c r="N41" t="inlineStr">
         <is>
@@ -4008,8 +4127,10 @@
           <t>1721102119136 - 13 - NAPOLES - CATALUÑA - W - 10:30</t>
         </is>
       </c>
-      <c r="D42" t="b">
-        <v>1</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -4045,10 +4166,10 @@
         <v>13</v>
       </c>
       <c r="L42" t="n">
+        <v>48</v>
+      </c>
+      <c r="M42" t="n">
         <v>5</v>
-      </c>
-      <c r="M42" t="n">
-        <v>48</v>
       </c>
       <c r="N42" t="inlineStr">
         <is>
@@ -4068,8 +4189,10 @@
           <t>1721101949589 - 14 - NAPOLES - VERDAGUER - 11:00</t>
         </is>
       </c>
-      <c r="D43" t="b">
-        <v>0</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -4105,10 +4228,10 @@
         <v>12</v>
       </c>
       <c r="L43" t="n">
+        <v>26</v>
+      </c>
+      <c r="M43" t="n">
         <v>2</v>
-      </c>
-      <c r="M43" t="n">
-        <v>26</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
@@ -4128,8 +4251,10 @@
           <t>1721102224478 - 16 - NAPOLES - BORN - 11:30</t>
         </is>
       </c>
-      <c r="D44" t="b">
-        <v>0</v>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -4165,10 +4290,10 @@
         <v>20</v>
       </c>
       <c r="L44" t="n">
+        <v>76</v>
+      </c>
+      <c r="M44" t="n">
         <v>8</v>
-      </c>
-      <c r="M44" t="n">
-        <v>76</v>
       </c>
       <c r="N44" t="inlineStr">
         <is>
@@ -4188,8 +4313,10 @@
           <t>1721102651888 - 15 - NAPOLES - GOTIC - 11:30</t>
         </is>
       </c>
-      <c r="D45" t="b">
-        <v>0</v>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -4225,10 +4352,10 @@
         <v>18</v>
       </c>
       <c r="L45" t="n">
+        <v>46</v>
+      </c>
+      <c r="M45" t="n">
         <v>4</v>
-      </c>
-      <c r="M45" t="n">
-        <v>46</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
@@ -4248,8 +4375,10 @@
           <t>1721102627472 - 17 - NAPOLES - GOTIC - 12:00</t>
         </is>
       </c>
-      <c r="D46" t="b">
-        <v>0</v>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -4285,10 +4414,10 @@
         <v>19</v>
       </c>
       <c r="L46" t="n">
+        <v>61</v>
+      </c>
+      <c r="M46" t="n">
         <v>6</v>
-      </c>
-      <c r="M46" t="n">
-        <v>61</v>
       </c>
       <c r="N46" t="inlineStr">
         <is>
@@ -4308,8 +4437,10 @@
           <t>1721102268642 - 18 - NAPOLES - PUERTO - 12:00</t>
         </is>
       </c>
-      <c r="D47" t="b">
-        <v>0</v>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -4345,10 +4476,10 @@
         <v>26</v>
       </c>
       <c r="L47" t="n">
+        <v>40</v>
+      </c>
+      <c r="M47" t="n">
         <v>2</v>
-      </c>
-      <c r="M47" t="n">
-        <v>40</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -4368,8 +4499,10 @@
           <t>1721102689216 - 19 - NAPOLES - TARDE - W - 17:00</t>
         </is>
       </c>
-      <c r="D48" t="b">
-        <v>1</v>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -4405,10 +4538,10 @@
         <v>12</v>
       </c>
       <c r="L48" t="n">
+        <v>19</v>
+      </c>
+      <c r="M48" t="n">
         <v>1</v>
-      </c>
-      <c r="M48" t="n">
-        <v>19</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -4447,7 +4580,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="J53" s="1" t="inlineStr">
@@ -4472,7 +4605,7 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>J</t>
         </is>
       </c>
       <c r="Q53" s="1" t="inlineStr">
@@ -4520,17 +4653,17 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>1721101666656</t>
+          <t>1721102082040</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>10:51</t>
+          <t>08:16</t>
         </is>
       </c>
       <c r="P54" s="1" t="n">
@@ -4538,17 +4671,17 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>1721102119136</t>
+          <t>1721101715356</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>10:20</t>
+          <t>07:50</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>11:18</t>
+          <t>08:52</t>
         </is>
       </c>
     </row>
@@ -4574,48 +4707,6 @@
       <c r="F55" t="n">
         <v>0</v>
       </c>
-      <c r="I55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>1721102651888</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>11:05</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>12:01</t>
-        </is>
-      </c>
-      <c r="M55" t="n">
-        <v>14</v>
-      </c>
-      <c r="P55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>1721102268642</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>11:35</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>12:15</t>
-        </is>
-      </c>
-      <c r="T55" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="56">
       <c r="B56" s="1" t="n">
@@ -4639,27 +4730,6 @@
       <c r="F56" t="n">
         <v>0</v>
       </c>
-      <c r="I56" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>1721102627472</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>12:01</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>13:02</t>
-        </is>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="57">
       <c r="B57" s="1" t="n">
@@ -4707,403 +4777,472 @@
         <v>0</v>
       </c>
     </row>
+    <row r="62">
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D62" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="J62" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="K62" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="L62" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="M62" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="Q62" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="R62" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="S62" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="T62" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+    </row>
     <row r="63">
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="C63" s="1" t="inlineStr">
+      <c r="B63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>1721101989601</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>07:50</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>1721102423348</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>07:50</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>08:37</t>
+        </is>
+      </c>
+      <c r="P63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>1721102462855</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>07:50</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>08:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D63" s="1" t="inlineStr">
+      <c r="D71" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E63" s="1" t="inlineStr">
+      <c r="E71" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F63" s="1" t="inlineStr">
+      <c r="F71" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="J63" s="1" t="inlineStr">
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="J71" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K63" s="1" t="inlineStr">
+      <c r="K71" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L63" s="1" t="inlineStr">
+      <c r="L71" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M63" s="1" t="inlineStr">
+      <c r="M71" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P63" t="inlineStr">
+      <c r="P71" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="Q63" s="1" t="inlineStr">
+      <c r="Q71" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="R63" s="1" t="inlineStr">
+      <c r="R71" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="S63" s="1" t="inlineStr">
+      <c r="S71" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="T63" s="1" t="inlineStr">
+      <c r="T71" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="B64" s="1" t="n">
+    <row r="72">
+      <c r="B72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>1721101715356</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>1721102486645</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
         <is>
           <t>07:50</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="I64" s="1" t="n">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>08:17</t>
+        </is>
+      </c>
+      <c r="I72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>1721101989601</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>07:50</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="P64" s="1" t="n">
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>1721101666656</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>10:51</t>
+        </is>
+      </c>
+      <c r="P72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q64" t="inlineStr">
+      <c r="Q72" t="inlineStr">
         <is>
           <t>1721102522098</t>
         </is>
       </c>
-      <c r="R64" t="inlineStr">
+      <c r="R72" t="inlineStr">
         <is>
           <t>09:50</t>
         </is>
       </c>
-      <c r="S64" t="inlineStr">
+      <c r="S72" t="inlineStr">
         <is>
           <t>10:37</t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="B72" t="inlineStr">
+    <row r="73">
+      <c r="I73" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>1721102651888</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="I74" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>1721102627472</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="C72" s="1" t="inlineStr">
+      <c r="C80" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D72" s="1" t="inlineStr">
+      <c r="D80" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E72" s="1" t="inlineStr">
+      <c r="E80" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F72" s="1" t="inlineStr">
+      <c r="F80" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="J72" s="1" t="inlineStr">
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="J80" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K72" s="1" t="inlineStr">
+      <c r="K80" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L72" s="1" t="inlineStr">
+      <c r="L80" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M72" s="1" t="inlineStr">
+      <c r="M80" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="Q72" s="1" t="inlineStr">
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="Q80" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="R72" s="1" t="inlineStr">
+      <c r="R80" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="S72" s="1" t="inlineStr">
+      <c r="S80" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="T72" s="1" t="inlineStr">
+      <c r="T80" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="B73" s="1" t="n">
+    <row r="81">
+      <c r="B81" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>1721102546874</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>09:50</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>10:38</t>
         </is>
       </c>
-      <c r="I73" s="1" t="n">
+      <c r="I81" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>1721102423348</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>07:50</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-      <c r="P73" s="1" t="n">
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>1721102119136</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>10:20</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>11:18</t>
+        </is>
+      </c>
+      <c r="P81" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>1721102462855</t>
-        </is>
-      </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>07:50</t>
-        </is>
-      </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="C81" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="D81" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="E81" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="F81" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J81" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="K81" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="L81" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="M81" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="Q81" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="R81" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="S81" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="T81" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>1721102689216</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>16:50</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>17:09</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="B82" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>1721102082040</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>07:35</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>08:16</t>
-        </is>
-      </c>
       <c r="I82" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>1721102486645</t>
+          <t>1721102268642</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>07:50</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>08:17</t>
-        </is>
-      </c>
-      <c r="P82" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>1721102689216</t>
-        </is>
-      </c>
-      <c r="R82" t="inlineStr">
-        <is>
-          <t>16:50</t>
-        </is>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>17:09</t>
-        </is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -5191,21 +5330,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>12:43</t>
+          <t>11:20</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="5">
@@ -5219,21 +5358,21 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11:20</t>
+          <t>12:43</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3.7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="6">
@@ -5247,21 +5386,21 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>I</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>08:38</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11:40</t>
+          <t>10:01</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="7">
@@ -5275,21 +5414,21 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10:01</t>
+          <t>11:40</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -5389,8 +5528,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19"/>
-    <row r="20"/>
+    <row r="15">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Trikes</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Percentatge Trikes</t>
+        </is>
+      </c>
+      <c r="G16">
+        <f>G15/G13</f>
+        <v/>
+      </c>
+    </row>
     <row r="21"/>
     <row r="22"/>
     <row r="23"/>
@@ -5402,7 +5560,7 @@
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Prioritari</t>
+          <t>Tipus Bici</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
@@ -5442,12 +5600,12 @@
       </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
+          <t>Temps Total Ruta</t>
+        </is>
+      </c>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
           <t>Num Entregues</t>
-        </is>
-      </c>
-      <c r="M24" s="1" t="inlineStr">
-        <is>
-          <t>Temps Total Ruta</t>
         </is>
       </c>
       <c r="N24" s="1" t="inlineStr">
@@ -5470,8 +5628,10 @@
           <t>1721100355845 - 01 - SANTS - NUMANCIA - 07:40</t>
         </is>
       </c>
-      <c r="D25" t="b">
-        <v>0</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -5507,10 +5667,10 @@
         <v>16</v>
       </c>
       <c r="L25" t="n">
+        <v>58</v>
+      </c>
+      <c r="M25" t="n">
         <v>6</v>
-      </c>
-      <c r="M25" t="n">
-        <v>58</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -5530,8 +5690,10 @@
           <t>1721100497594 - 02 - SANTS - TARRADELLAS - 08:00</t>
         </is>
       </c>
-      <c r="D26" t="b">
-        <v>0</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5567,10 +5729,10 @@
         <v>16</v>
       </c>
       <c r="L26" t="n">
+        <v>37</v>
+      </c>
+      <c r="M26" t="n">
         <v>3</v>
-      </c>
-      <c r="M26" t="n">
-        <v>37</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -5590,8 +5752,10 @@
           <t>1721100630101 - 04 - SANTS - BERLIN - 08:30</t>
         </is>
       </c>
-      <c r="D27" t="b">
-        <v>0</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5627,10 +5791,10 @@
         <v>16</v>
       </c>
       <c r="L27" t="n">
+        <v>37</v>
+      </c>
+      <c r="M27" t="n">
         <v>3</v>
-      </c>
-      <c r="M27" t="n">
-        <v>37</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -5650,8 +5814,10 @@
           <t>1721101262949 - 03 - SANTS - RAVAL - 08:30</t>
         </is>
       </c>
-      <c r="D28" t="b">
-        <v>0</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5687,10 +5853,10 @@
         <v>17</v>
       </c>
       <c r="L28" t="n">
+        <v>31</v>
+      </c>
+      <c r="M28" t="n">
         <v>2</v>
-      </c>
-      <c r="M28" t="n">
-        <v>31</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -5710,8 +5876,10 @@
           <t>1721100247896 - 05 - SANTS - ROCAFORT - W - 08:45</t>
         </is>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5747,10 +5915,10 @@
         <v>15</v>
       </c>
       <c r="L29" t="n">
+        <v>50</v>
+      </c>
+      <c r="M29" t="n">
         <v>5</v>
-      </c>
-      <c r="M29" t="n">
-        <v>50</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
@@ -5770,8 +5938,10 @@
           <t>1721100922012 - 06 - SANTS - SANT RAMON - W - 09:00</t>
         </is>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5807,10 +5977,10 @@
         <v>31</v>
       </c>
       <c r="L30" t="n">
+        <v>66</v>
+      </c>
+      <c r="M30" t="n">
         <v>5</v>
-      </c>
-      <c r="M30" t="n">
-        <v>66</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -5830,8 +6000,10 @@
           <t>1721100178035 - 07 - SANTS - GOTIC - W - 09:20</t>
         </is>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5867,10 +6039,10 @@
         <v>25</v>
       </c>
       <c r="L31" t="n">
+        <v>67</v>
+      </c>
+      <c r="M31" t="n">
         <v>6</v>
-      </c>
-      <c r="M31" t="n">
-        <v>67</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -5890,8 +6062,10 @@
           <t>1721101127690 - 08 - SANTS - CLINIC - W - 09:30</t>
         </is>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5927,10 +6101,10 @@
         <v>14</v>
       </c>
       <c r="L32" t="n">
+        <v>35</v>
+      </c>
+      <c r="M32" t="n">
         <v>3</v>
-      </c>
-      <c r="M32" t="n">
-        <v>35</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -5950,8 +6124,10 @@
           <t>1721100593141 - 09 - SANTS - NUMANCIA - 09:30</t>
         </is>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -5987,10 +6163,10 @@
         <v>19</v>
       </c>
       <c r="L33" t="n">
+        <v>54</v>
+      </c>
+      <c r="M33" t="n">
         <v>5</v>
-      </c>
-      <c r="M33" t="n">
-        <v>54</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
@@ -6010,8 +6186,10 @@
           <t>1721100704935 - 12 - SANTS - CLINIC - W - 10:00</t>
         </is>
       </c>
-      <c r="D34" t="b">
-        <v>1</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6047,10 +6225,10 @@
         <v>21</v>
       </c>
       <c r="L34" t="n">
+        <v>63</v>
+      </c>
+      <c r="M34" t="n">
         <v>6</v>
-      </c>
-      <c r="M34" t="n">
-        <v>63</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
@@ -6070,8 +6248,10 @@
           <t>1721101164491 - 11 - SANTS - SANT ANTONI - W - 10:00</t>
         </is>
       </c>
-      <c r="D35" t="b">
-        <v>1</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -6107,10 +6287,10 @@
         <v>19</v>
       </c>
       <c r="L35" t="n">
+        <v>54</v>
+      </c>
+      <c r="M35" t="n">
         <v>5</v>
-      </c>
-      <c r="M35" t="n">
-        <v>54</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
@@ -6130,8 +6310,10 @@
           <t>1721101394043 - 10 - S01 - SANTS - SYNLAB - 10:00</t>
         </is>
       </c>
-      <c r="D36" t="b">
-        <v>0</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6167,10 +6349,10 @@
         <v>84</v>
       </c>
       <c r="L36" t="n">
+        <v>119</v>
+      </c>
+      <c r="M36" t="n">
         <v>5</v>
-      </c>
-      <c r="M36" t="n">
-        <v>119</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
@@ -6190,8 +6372,10 @@
           <t>1721101237043 - 13 - SANTS - GOTIC - 10:30</t>
         </is>
       </c>
-      <c r="D37" t="b">
-        <v>0</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -6227,10 +6411,10 @@
         <v>19</v>
       </c>
       <c r="L37" t="n">
+        <v>40</v>
+      </c>
+      <c r="M37" t="n">
         <v>3</v>
-      </c>
-      <c r="M37" t="n">
-        <v>40</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
@@ -6250,8 +6434,10 @@
           <t>1721100447653 - 15 - SANTS - GOTIC - 11:00</t>
         </is>
       </c>
-      <c r="D38" t="b">
-        <v>0</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -6287,10 +6473,10 @@
         <v>23</v>
       </c>
       <c r="L38" t="n">
+        <v>51</v>
+      </c>
+      <c r="M38" t="n">
         <v>4</v>
-      </c>
-      <c r="M38" t="n">
-        <v>51</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
@@ -6310,8 +6496,10 @@
           <t>1721101195978 - 14 - SANTS - ENTENÇA - 11:00</t>
         </is>
       </c>
-      <c r="D39" t="b">
-        <v>0</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4 wheels</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -6347,10 +6535,10 @@
         <v>11</v>
       </c>
       <c r="L39" t="n">
+        <v>32</v>
+      </c>
+      <c r="M39" t="n">
         <v>3</v>
-      </c>
-      <c r="M39" t="n">
-        <v>32</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -6370,8 +6558,10 @@
           <t>1721101020078 - 16 - SANTS - ARIBAU - W - 12:00</t>
         </is>
       </c>
-      <c r="D40" t="b">
-        <v>1</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -6407,10 +6597,10 @@
         <v>20</v>
       </c>
       <c r="L40" t="n">
+        <v>48</v>
+      </c>
+      <c r="M40" t="n">
         <v>4</v>
-      </c>
-      <c r="M40" t="n">
-        <v>48</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
@@ -6430,8 +6620,10 @@
           <t>1721101422578 - 17 - S02 - SANTS - SYNLAB - 13:00</t>
         </is>
       </c>
-      <c r="D41" t="b">
-        <v>0</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -6467,10 +6659,10 @@
         <v>68</v>
       </c>
       <c r="L41" t="n">
+        <v>89</v>
+      </c>
+      <c r="M41" t="n">
         <v>3</v>
-      </c>
-      <c r="M41" t="n">
-        <v>89</v>
       </c>
       <c r="N41" t="inlineStr">
         <is>
@@ -6490,8 +6682,10 @@
           <t>1721101452774 - 18 - S03 - SANTS - SYNLAB - 16:00</t>
         </is>
       </c>
-      <c r="D42" t="b">
-        <v>0</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -6527,10 +6721,10 @@
         <v>88</v>
       </c>
       <c r="L42" t="n">
+        <v>123</v>
+      </c>
+      <c r="M42" t="n">
         <v>5</v>
-      </c>
-      <c r="M42" t="n">
-        <v>123</v>
       </c>
       <c r="N42" t="inlineStr">
         <is>
@@ -6550,8 +6744,10 @@
           <t>1721101486211 - 19 - S04 - SANTS - SYNLAB - 18:00</t>
         </is>
       </c>
-      <c r="D43" t="b">
-        <v>0</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Trike</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -6587,10 +6783,10 @@
         <v>69</v>
       </c>
       <c r="L43" t="n">
+        <v>90</v>
+      </c>
+      <c r="M43" t="n">
         <v>3</v>
-      </c>
-      <c r="M43" t="n">
-        <v>90</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
@@ -6629,32 +6825,32 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="J48" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="K48" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="L48" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="M48" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
           <t>C</t>
-        </is>
-      </c>
-      <c r="J48" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="K48" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="L48" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="M48" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>E</t>
         </is>
       </c>
       <c r="Q48" s="1" t="inlineStr">
@@ -6702,17 +6898,17 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>1721100247896</t>
+          <t>1721100497594</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>07:50</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="P49" s="1" t="n">
@@ -6720,17 +6916,17 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>1721100497594</t>
+          <t>1721100247896</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>07:50</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>08:37</t>
+          <t>09:35</t>
         </is>
       </c>
     </row>
@@ -6761,17 +6957,17 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>1721100593141</t>
+          <t>1721101262949</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>10:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="M50" t="n">
@@ -6782,17 +6978,17 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>1721101262949</t>
+          <t>1721100593141</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>08:37</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>10:39</t>
         </is>
       </c>
       <c r="T50" t="n">
@@ -6826,17 +7022,17 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>1721100447653</t>
+          <t>1721100178035</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>10:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>11:40</t>
+          <t>10:35</t>
         </is>
       </c>
       <c r="M51" t="n">
@@ -6847,17 +7043,17 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>1721100178035</t>
+          <t>1721100447653</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>10:39</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>10:35</t>
+          <t>11:40</t>
         </is>
       </c>
       <c r="T51" t="n">
@@ -6891,42 +7087,42 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>1721101020078</t>
+          <t>1721101237043</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>11:50</t>
+          <t>10:35</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P52" s="1" t="n">
         <v>3</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>1721101237043</t>
+          <t>1721101020078</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>10:35</t>
+          <t>11:50</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="T52" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53">
@@ -6955,32 +7151,32 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
           <t>H</t>
-        </is>
-      </c>
-      <c r="C60" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="D60" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="E60" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="F60" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>I</t>
         </is>
       </c>
       <c r="J60" s="1" t="inlineStr">
@@ -7035,17 +7231,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1721100704935</t>
+          <t>1721100922012</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>09:56</t>
         </is>
       </c>
       <c r="I61" s="1" t="n">
@@ -7053,17 +7249,17 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>1721100922012</t>
+          <t>1721100704935</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>09:50</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>09:56</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="P61" s="1" t="n">
@@ -7086,25 +7282,25 @@
       </c>
     </row>
     <row r="62">
-      <c r="B62" s="1" t="n">
+      <c r="I62" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="J62" t="inlineStr">
         <is>
           <t>1721101195978</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="K62" t="inlineStr">
         <is>
           <t>11:03</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="L62" t="inlineStr">
         <is>
           <t>11:35</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="M62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7189,7 +7385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7337,6 +7533,16 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Pes Trike</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
horaris funciona i afegit info extre tipus de bici
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2905,6 +2905,26 @@
           <t>Hores Totals</t>
         </is>
       </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Treballador</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Sortida</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Hores</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="n">
@@ -2933,6 +2953,24 @@
       <c r="G3" t="n">
         <v>5.3</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>7:45</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="n">
@@ -2961,6 +2999,24 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Fede Goss</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8:15</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n">
@@ -2989,6 +3045,24 @@
       <c r="G5" t="n">
         <v>1.3</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Gianluca</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="n">
@@ -3017,6 +3091,24 @@
       <c r="G6" t="n">
         <v>1.3</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Laila</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="n">
@@ -3045,6 +3137,24 @@
       <c r="G7" t="n">
         <v>1.1</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Vladi</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>9:15</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n">
@@ -3073,6 +3183,24 @@
       <c r="G8" t="n">
         <v>1.1</v>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Erick</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>9:45</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="n">
@@ -3101,6 +3229,24 @@
       <c r="G9" t="n">
         <v>0.7</v>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Sebastián</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="n">
@@ -3243,68 +3389,83 @@
       </c>
     </row>
     <row r="16">
-      <c r="F16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="G16">
+      <c r="F16">
         <f>SUM(G3:G14)</f>
         <v/>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Total Hores</t>
+        </is>
+      </c>
+      <c r="L16">
+        <f>SUM(L3:L15)</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
-      <c r="F17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Num treballadors</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="F17" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="18">
-      <c r="F18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Num Rutes</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="F18" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="19">
-      <c r="F19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Total Paquets</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="F19" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="20">
-      <c r="F20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Trikes</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="F20" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Percentatge Trikes</t>
-        </is>
-      </c>
-      <c r="G21">
+      <c r="G20">
         <f>G20/G18</f>
         <v/>
       </c>
     </row>
-    <row r="26"/>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>4 Wheeler</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <f>G21/G18</f>
+        <v/>
+      </c>
+    </row>
     <row r="27"/>
     <row r="28"/>
     <row r="29">
@@ -5290,6 +5451,26 @@
           <t>Hores Totals</t>
         </is>
       </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Treballador</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Sortida</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Hores</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="n">
@@ -5318,6 +5499,24 @@
       <c r="G3" t="n">
         <v>6.8</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Jordi</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="n">
@@ -5346,6 +5545,24 @@
       <c r="G4" t="n">
         <v>3.7</v>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Rocco</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>7:45</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n">
@@ -5374,6 +5591,24 @@
       <c r="G5" t="n">
         <v>4.3</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Alejandro</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="n">
@@ -5402,6 +5637,24 @@
       <c r="G6" t="n">
         <v>1.4</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Hans</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>9:30</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="n">
@@ -5430,6 +5683,24 @@
       <c r="G7" t="n">
         <v>2</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Jaime</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n">
@@ -5458,6 +5729,24 @@
       <c r="G8" t="n">
         <v>1.2</v>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="n">
@@ -5488,68 +5777,83 @@
       </c>
     </row>
     <row r="11">
-      <c r="F11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="G11">
+      <c r="F11">
         <f>SUM(G3:G9)</f>
         <v/>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Total Hores</t>
+        </is>
+      </c>
+      <c r="L11">
+        <f>SUM(L3:L10)</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
-      <c r="F12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Num treballadors</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="F12" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="13">
-      <c r="F13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Num Rutes</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="F13" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="14">
-      <c r="F14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Total Paquets</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="15">
-      <c r="F15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Trikes</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="F15" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Percentatge Trikes</t>
-        </is>
-      </c>
-      <c r="G16">
+      <c r="G15">
         <f>G15/G13</f>
         <v/>
       </c>
     </row>
-    <row r="21"/>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4 Wheeler</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <f>G16/G13</f>
+        <v/>
+      </c>
+    </row>
     <row r="22"/>
     <row r="23"/>
     <row r="24">

</xml_diff>

<commit_message>
Added efficient bike distribution number
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2909,26 +2909,6 @@
           <t>Hores Totals</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>Treballador</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>Entrada</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>Sortida</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Hores</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="n">
@@ -2957,24 +2937,6 @@
       <c r="G3" t="n">
         <v>5.3</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Zoe</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>7:45</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>13:45</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="n">
@@ -3003,24 +2965,6 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Fede Goss</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>8:15</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>12:15</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n">
@@ -3049,24 +2993,6 @@
       <c r="G5" t="n">
         <v>1.3</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Gianluca</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>8:30</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>12:30</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="n">
@@ -3095,24 +3021,6 @@
       <c r="G6" t="n">
         <v>1.3</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Laila</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>9:00</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="n">
@@ -3141,24 +3049,6 @@
       <c r="G7" t="n">
         <v>1.1</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Vladi</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>9:15</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>16:15</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n">
@@ -3187,24 +3077,6 @@
       <c r="G8" t="n">
         <v>1.1</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Erick</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>9:45</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>12:15</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="n">
@@ -3233,24 +3105,6 @@
       <c r="G9" t="n">
         <v>0.7</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Sebastián</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="n">
@@ -3470,8 +3324,26 @@
         <v/>
       </c>
     </row>
-    <row r="27"/>
-    <row r="28"/>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Trikes Min En Hub</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>4 Wheeler Min En Hub</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>5</v>
+      </c>
+    </row>
     <row r="29">
       <c r="C29" s="1" t="inlineStr">
         <is>
@@ -5455,26 +5327,6 @@
           <t>Hores Totals</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>Treballador</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>Entrada</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>Sortida</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Hores</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="n">
@@ -5503,24 +5355,6 @@
       <c r="G3" t="n">
         <v>6.8</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Jordi</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>7:30</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>12:30</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="n">
@@ -5549,24 +5383,6 @@
       <c r="G4" t="n">
         <v>3.7</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Rocco</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>7:45</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>4.3</v>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="n">
@@ -5595,24 +5411,6 @@
       <c r="G5" t="n">
         <v>4.3</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Alejandro</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>8:00</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="n">
@@ -5641,24 +5439,6 @@
       <c r="G6" t="n">
         <v>1.4</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Hans</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>9:30</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="n">
@@ -5687,24 +5467,6 @@
       <c r="G7" t="n">
         <v>2</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Jaime</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n">
@@ -5733,24 +5495,6 @@
       <c r="G8" t="n">
         <v>1.2</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Diego</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="n">
@@ -5858,8 +5602,26 @@
         <v/>
       </c>
     </row>
-    <row r="22"/>
-    <row r="23"/>
+    <row r="17">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Trikes Min En Hub</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4 Wheeler Min En Hub</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>3</v>
+      </c>
+    </row>
     <row r="24">
       <c r="C24" s="1" t="inlineStr">
         <is>
@@ -7101,7 +6863,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="O43" t="n">
+      <c r="O43" s="2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nou parche per al nou format
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,11 +534,11 @@
     </row>
     <row r="3">
       <c r="B3" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1730183168707 - 02 - NAPOLES - GOTIC - W - 08:30</t>
+          <t>1731998803597 - 01 - NAPOLES - GOTIC - 08:30</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -547,11 +547,11 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -571,26 +571,26 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>09:37</t>
+          <t>10:47</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09:47</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="M3" t="n">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="N3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -599,24 +599,24 @@
     </row>
     <row r="4">
       <c r="B4" s="1" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1730182013914 - 01 - NAPOLES - DIAGONAL - W - 08:30</t>
+          <t>1731999790486 - 06 - NAPOLES - GOTIC - 10:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TRIKE</t>
+          <t>4W</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -626,36 +626,36 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>8:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>08:20</t>
+          <t>09:50</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>10:17</t>
+          <t>12:11</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="M4" t="n">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="N4" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>K</t>
         </is>
       </c>
       <c r="P4" t="n">
@@ -664,11 +664,11 @@
     </row>
     <row r="5">
       <c r="B5" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1730183826011 - 05 - NAPOLES - P9 - W - ! - 10:00</t>
+          <t>1731999205451 - 03 - NAPOLES - SAGRERA - W - 10:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -701,26 +701,26 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>13:29</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="M5" t="n">
-        <v>102</v>
+        <v>209</v>
       </c>
       <c r="N5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -733,7 +733,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1730183577969 - 03 - NAPOLES - DIAGONAL - W - 10:00</t>
+          <t>1731999042123 - 02 - NAPOLES - P9 - W - 10:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -742,11 +742,11 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -766,19 +766,19 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>11:36</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="M6" t="n">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="N6" t="n">
         <v>10</v>
@@ -794,11 +794,11 @@
     </row>
     <row r="7">
       <c r="B7" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1730183671543 - 04 - NAPOLES - CATALUNYA - W - 10:00</t>
+          <t>1731999265927 - 04 - NAPOLES - TETUAN - W - 11:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -807,11 +807,11 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -821,49 +821,49 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>11:17</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="M7" t="n">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="N7" t="n">
         <v>9</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>-10</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1730184365016 - 07 - NAPOLES - GOTIC - W - 11:00</t>
+          <t>1731999825299 - 07 - NAPOLES - DIAGONAL - 11:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -872,11 +872,11 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -896,26 +896,26 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>14:08</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="M8" t="n">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="N8" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>G</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -928,7 +928,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1730184302467 - 06 - NAPOLES - PASSEIG DE GRACIA11:00</t>
+          <t>1731999561009 - 05 - NAPOLES - ENRIC GRANADOS - 11:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -937,11 +937,11 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -956,44 +956,44 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10:35</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>11:37</t>
+          <t>14:08</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>11:47</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="M9" t="n">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="N9" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>-25</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1730184427958 - 08 - NAPOLES - TARDE - 16:00</t>
+          <t>1732000039740 - 08 - NAPOLES - TARDE - 15:30</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1016,36 +1016,36 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>18:07</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="M10" t="n">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>H</t>
         </is>
       </c>
       <c r="P10" t="n">
@@ -1054,11 +1054,11 @@
     </row>
     <row r="11">
       <c r="B11" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1730184739357 - 01 - SANTS - SANT - ANTONI - W -09:00</t>
+          <t>1732000314215 - 01 - SANTS - ESTACIO - W - 09:30</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1067,11 +1067,11 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1081,36 +1081,36 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>9:00</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>10:20</t>
+          <t>11:36</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="M11" t="n">
-        <v>80</v>
+        <v>126</v>
       </c>
       <c r="N11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -1119,11 +1119,11 @@
     </row>
     <row r="12">
       <c r="B12" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1730184819693 - 02 - SANTS - LES CORTS - W - 10:00</t>
+          <t>1732000504888 - 02 - SANTS - DIAGONAL - 10:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1132,11 +1132,11 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1156,26 +1156,26 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>11:44</t>
+          <t>12:23</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="M12" t="n">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="N12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -1184,11 +1184,11 @@
     </row>
     <row r="13">
       <c r="B13" s="1" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1730184488854 - S01 - SANTS - SYNLAB - 10:00</t>
+          <t>1731998556866 - S01 - SANTS - SYNLAB - 10:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1221,26 +1221,26 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>11:48</t>
+          <t>12:19</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="M13" t="n">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>J</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1249,11 +1249,11 @@
     </row>
     <row r="14">
       <c r="B14" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1730184584024 - S02 - SANTS - SYNLAB - 13:00</t>
+          <t>1732000594042 - 03 - SANTS - URGELL 10:30</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1262,11 +1262,11 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1276,36 +1276,36 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>10:20</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>12:57</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="M14" t="n">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="N14" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>I</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -1314,11 +1314,11 @@
     </row>
     <row r="15">
       <c r="B15" s="1" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1730185133340 - 03 - SANTS - TARDE - W - 15:30</t>
+          <t>1731998598378 - S02 - SANTS - SYNLAB - 13:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1327,11 +1327,11 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1341,49 +1341,49 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>14:23</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M15" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="N15" t="n">
         <v>3</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>-10</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1730184635223 - S03 - SANTS - SYNLAB - 16:30</t>
+          <t>1732000704516 - 04 - SANTS - TARDE - W - 15:30</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1392,57 +1392,122 @@
         </is>
       </c>
       <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sants</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>46</v>
+      </c>
+      <c r="M16" t="n">
+        <v>74</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1731998639325 - S03 - SANTS - SYNLAB - 16:30</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>TRIKE</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>24</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>29/10/2024</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Sants</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>16:24</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>18:31</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>18:41</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>85</v>
-      </c>
-      <c r="M16" t="n">
-        <v>127</v>
-      </c>
-      <c r="N16" t="n">
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>125</v>
+      </c>
+      <c r="M17" t="n">
+        <v>167</v>
+      </c>
+      <c r="N17" t="n">
         <v>6</v>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="P16" t="n">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="17"/>
+      <c r="P17" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1454,7 +1519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,11 +1598,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="4">
@@ -1551,21 +1616,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08:08</t>
+          <t>09:38</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11:37</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="5">
@@ -1589,11 +1654,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>13:05</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="6">
@@ -1607,7 +1672,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>K</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1617,11 +1682,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11:22</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.7</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="7">
@@ -1635,7 +1700,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1645,11 +1710,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>14:13</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.4</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="8">
@@ -1663,269 +1728,232 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>10:38</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>16:59</t>
+          <t>14:03</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="9"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Napoles</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>15:08</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>18:12</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
     <row r="10"/>
-    <row r="11">
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Total Hores</t>
-        </is>
-      </c>
-      <c r="F11">
-        <f>SUM(G3:G8)</f>
-        <v/>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Total Hores</t>
-        </is>
-      </c>
-      <c r="L11">
-        <f>SUM(L3:L10)</f>
-        <v/>
-      </c>
-    </row>
+    <row r="11"/>
     <row r="12">
       <c r="E12" t="inlineStr">
         <is>
-          <t>Num treballadors</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
+          <t>Total Hores</t>
+        </is>
+      </c>
+      <c r="F12">
+        <f>SUM(G3:G9)</f>
+        <v/>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Total Hores</t>
+        </is>
+      </c>
+      <c r="L12">
+        <f>SUM(L3:L11)</f>
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="E13" t="inlineStr">
         <is>
-          <t>Num Rutes</t>
+          <t>Num treballadors</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>TRIKES</t>
-        </is>
-      </c>
-      <c r="J13" t="n">
-        <v>8</v>
-      </c>
-      <c r="K13" s="2">
-        <f>J13/F13</f>
-        <v/>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
+          <t>Num Rutes</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>TRIKES</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>7</v>
+      </c>
+      <c r="K14" s="2">
+        <f>J14/F14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Total Paquets</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>60</v>
-      </c>
-      <c r="I14" t="inlineStr">
+      <c r="F15" t="n">
+        <v>80</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>4W</t>
         </is>
       </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <f>J14/F13</f>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <f>J15/F14</f>
         <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>TRIKES Min</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="I16" t="inlineStr">
         <is>
+          <t>TRIKES Min</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="I17" t="inlineStr">
+        <is>
           <t>4w  Min</t>
         </is>
       </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17"/>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="18"/>
     <row r="19"/>
     <row r="20"/>
     <row r="21"/>
     <row r="22"/>
-    <row r="23">
-      <c r="C23" s="1" t="inlineStr">
+    <row r="23"/>
+    <row r="24">
+      <c r="C24" s="1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="D23" s="1" t="inlineStr">
+      <c r="D24" s="1" t="inlineStr">
         <is>
           <t>Tipus Bici</t>
         </is>
       </c>
-      <c r="E23" s="1" t="inlineStr">
+      <c r="E24" s="1" t="inlineStr">
         <is>
           <t>Pes</t>
         </is>
       </c>
-      <c r="F23" s="1" t="inlineStr">
+      <c r="F24" s="1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="G23" s="1" t="inlineStr">
+      <c r="G24" s="1" t="inlineStr">
         <is>
           <t>Hub</t>
         </is>
       </c>
-      <c r="H23" s="1" t="inlineStr">
+      <c r="H24" s="1" t="inlineStr">
         <is>
           <t>Hora Inici Ruta Plnif</t>
         </is>
       </c>
-      <c r="I23" s="1" t="inlineStr">
+      <c r="I24" s="1" t="inlineStr">
         <is>
           <t>Hora Inici Ruta Real</t>
         </is>
       </c>
-      <c r="J23" s="1" t="inlineStr">
+      <c r="J24" s="1" t="inlineStr">
         <is>
           <t>Hora Fi Ruta</t>
         </is>
       </c>
-      <c r="K23" s="1" t="inlineStr">
+      <c r="K24" s="1" t="inlineStr">
         <is>
           <t>Inici Seguent Ruta</t>
         </is>
       </c>
-      <c r="L23" s="1" t="inlineStr">
+      <c r="L24" s="1" t="inlineStr">
         <is>
           <t>Temps Recorregut Ruta</t>
         </is>
       </c>
-      <c r="M23" s="1" t="inlineStr">
+      <c r="M24" s="1" t="inlineStr">
         <is>
           <t>Temps Total Ruta</t>
         </is>
       </c>
-      <c r="N23" s="1" t="inlineStr">
+      <c r="N24" s="1" t="inlineStr">
         <is>
           <t>Num Entregues</t>
         </is>
       </c>
-      <c r="O23" s="1" t="inlineStr">
+      <c r="O24" s="1" t="inlineStr">
         <is>
           <t>Assignació</t>
         </is>
       </c>
-      <c r="P23" s="1" t="inlineStr">
+      <c r="P24" s="1" t="inlineStr">
         <is>
           <t>Plnif vs Real Min</t>
         </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>1730183168707 - 02 - NAPOLES - GOTIC - W - 08:30</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>TRIKE</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>18</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>29/10/2024</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Napoles</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>8:30</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>08:20</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>09:37</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>09:47</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>21</v>
-      </c>
-      <c r="M24" t="n">
-        <v>77</v>
-      </c>
-      <c r="N24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="P24" t="n">
-        <v>-10</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1730182013914 - 01 - NAPOLES - DIAGONAL - W - 08:30</t>
+          <t>1731998803597 - 01 - NAPOLES - GOTIC - 08:30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1934,11 +1962,11 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1958,22 +1986,22 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>10:17</t>
+          <t>10:47</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="M25" t="n">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="N25" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1986,24 +2014,24 @@
     </row>
     <row r="26">
       <c r="B26" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1730183826011 - 05 - NAPOLES - P9 - W - ! - 10:00</t>
+          <t>1731999790486 - 06 - NAPOLES - GOTIC - 10:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TRIKE</t>
+          <t>4W</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2023,26 +2051,26 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>12:11</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="M26" t="n">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="N26" t="n">
         <v>8</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>K</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -2051,11 +2079,11 @@
     </row>
     <row r="27">
       <c r="B27" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1730183577969 - 03 - NAPOLES - DIAGONAL - W - 10:00</t>
+          <t>1731999205451 - 03 - NAPOLES - SAGRERA - W - 10:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2064,11 +2092,11 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2088,26 +2116,26 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>11:36</t>
+          <t>13:29</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="M27" t="n">
-        <v>96</v>
+        <v>209</v>
       </c>
       <c r="N27" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -2116,11 +2144,11 @@
     </row>
     <row r="28">
       <c r="B28" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1730183671543 - 04 - NAPOLES - CATALUNYA - W - 10:00</t>
+          <t>1731999042123 - 02 - NAPOLES - P9 - W - 10:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2129,11 +2157,11 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2153,26 +2181,26 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>11:17</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="M28" t="n">
-        <v>87</v>
+        <v>190</v>
       </c>
       <c r="N28" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -2181,11 +2209,11 @@
     </row>
     <row r="29">
       <c r="B29" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1730184365016 - 07 - NAPOLES - GOTIC - W - 11:00</t>
+          <t>1731999265927 - 04 - NAPOLES - TETUAN - W - 11:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2194,11 +2222,11 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2213,44 +2241,44 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>10:50</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="M29" t="n">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="N29" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P29" t="n">
-        <v>-10</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1730184302467 - 06 - NAPOLES - PASSEIG DE GRACIA11:00</t>
+          <t>1731999825299 - 07 - NAPOLES - DIAGONAL - 11:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2259,11 +2287,11 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2278,44 +2306,44 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>10:35</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>11:37</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>11:47</t>
+          <t>14:08</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="M30" t="n">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="N30" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>G</t>
         </is>
       </c>
       <c r="P30" t="n">
-        <v>-25</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1730184427958 - 08 - NAPOLES - TARDE - 16:00</t>
+          <t>1731999561009 - 05 - NAPOLES - ENRIC GRANADOS - 11:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2324,11 +2352,11 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2338,359 +2366,457 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>14:08</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="M31" t="n">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="N31" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>E</t>
         </is>
       </c>
       <c r="P31" t="n">
         <v>-10</v>
       </c>
     </row>
-    <row r="32"/>
+    <row r="32">
+      <c r="B32" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1732000039740 - 08 - NAPOLES - TARDE - 15:30</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TRIKE</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Napoles</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>18:07</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="L32" t="n">
+        <v>104</v>
+      </c>
+      <c r="M32" t="n">
+        <v>167</v>
+      </c>
+      <c r="N32" t="n">
+        <v>9</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>-10</v>
+      </c>
+    </row>
     <row r="33"/>
     <row r="34"/>
     <row r="35"/>
-    <row r="36">
-      <c r="B36" t="inlineStr">
+    <row r="36"/>
+    <row r="37">
+      <c r="B37" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C36" s="1" t="inlineStr">
+      <c r="C37" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D36" s="1" t="inlineStr">
+      <c r="D37" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E36" s="1" t="inlineStr">
+      <c r="E37" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F36" s="1" t="inlineStr">
+      <c r="F37" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="J36" s="1" t="inlineStr">
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J37" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K36" s="1" t="inlineStr">
+      <c r="K37" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L36" s="1" t="inlineStr">
+      <c r="L37" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M36" s="1" t="inlineStr">
+      <c r="M37" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="Q36" s="1" t="inlineStr">
+      <c r="Q37" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="R36" s="1" t="inlineStr">
+      <c r="R37" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="S36" s="1" t="inlineStr">
+      <c r="S37" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="T36" s="1" t="inlineStr">
+      <c r="T37" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>1730182013914</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>08:20</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>10:27</t>
-        </is>
-      </c>
-      <c r="I37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>1730183168707</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>08:20</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>09:47</t>
-        </is>
-      </c>
-      <c r="P37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>1730183577969</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>09:50</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>11:26</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1731998803597</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>08:20</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>1731999205451</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>1731999042123</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1730184302467</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>10:35</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>11:37</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>8</v>
-      </c>
-      <c r="I38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>1730183826011</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>09:50</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>11:32</t>
-        </is>
-      </c>
-      <c r="M38" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1731999265927</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="40"/>
     <row r="41"/>
     <row r="42"/>
     <row r="43"/>
     <row r="44"/>
-    <row r="45">
-      <c r="B45" t="inlineStr">
+    <row r="45"/>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="J46" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="K46" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="L46" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="M46" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="C45" s="1" t="inlineStr">
+      <c r="Q46" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D45" s="1" t="inlineStr">
+      <c r="R46" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E45" s="1" t="inlineStr">
+      <c r="S46" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F45" s="1" t="inlineStr">
+      <c r="T46" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="J45" s="1" t="inlineStr">
+    </row>
+    <row r="47">
+      <c r="B47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1731999790486</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>12:11</t>
+        </is>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>1731999561009</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>10:50</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="P47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>1731999825299</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>10:50</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>13:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K45" s="1" t="inlineStr">
+      <c r="D55" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L45" s="1" t="inlineStr">
+      <c r="E55" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M45" s="1" t="inlineStr">
+      <c r="F55" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="Q45" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="R45" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="S45" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="T45" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="1" t="n">
+    </row>
+    <row r="56">
+      <c r="B56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1730183671543</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>09:50</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>11:17</t>
-        </is>
-      </c>
-      <c r="I46" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>1730184365016</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>10:50</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="P46" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>1730184427958</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>16:20</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>16:54</t>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1732000039740</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>18:07</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2715,7 +2841,7 @@
   <cols>
     <col width="2" customWidth="1" min="1" max="1"/>
     <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="55" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
@@ -2774,21 +2900,21 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10:15</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="4">
@@ -2802,7 +2928,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2812,11 +2938,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="5">
@@ -2830,7 +2956,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>J</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2840,11 +2966,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11:39</t>
+          <t>12:24</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="6">
@@ -2858,21 +2984,21 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>I</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>10:08</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>14:22</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.7</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="7">
@@ -2896,11 +3022,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="8"/>
@@ -2942,7 +3068,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -2950,7 +3076,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K12" s="2">
         <f>J12/F12</f>
@@ -2964,7 +3090,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -2986,7 +3112,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -3083,7 +3209,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1730184739357 - 01 - SANTS - SANT - ANTONI - W -09:00</t>
+          <t>1732000314215 - 01 - SANTS - ESTACIO - W - 09:30</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -3092,11 +3218,11 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3106,36 +3232,36 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>9:00</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>10:20</t>
+          <t>11:36</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="M23" t="n">
-        <v>80</v>
+        <v>126</v>
       </c>
       <c r="N23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -3148,7 +3274,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1730184819693 - 02 - SANTS - LES CORTS - W - 10:00</t>
+          <t>1732000504888 - 02 - SANTS - DIAGONAL - 10:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -3157,11 +3283,11 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -3181,26 +3307,26 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>11:44</t>
+          <t>12:23</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="M24" t="n">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="N24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -3213,7 +3339,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1730184488854 - S01 - SANTS - SYNLAB - 10:00</t>
+          <t>1731998556866 - S01 - SANTS - SYNLAB - 10:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3226,7 +3352,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -3246,26 +3372,26 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>11:48</t>
+          <t>12:19</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>12:29</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="M25" t="n">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="N25" t="n">
         <v>5</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>J</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -3278,7 +3404,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1730184584024 - S02 - SANTS - SYNLAB - 13:00</t>
+          <t>1732000594042 - 03 - SANTS - URGELL 10:30</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -3287,11 +3413,11 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -3301,36 +3427,36 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>10:20</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>12:57</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="M26" t="n">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="N26" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>I</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -3343,7 +3469,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1730185133340 - 03 - SANTS - TARDE - W - 15:30</t>
+          <t>1731998598378 - S02 - SANTS - SYNLAB - 13:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -3352,11 +3478,11 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3366,40 +3492,40 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>14:23</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M27" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="N27" t="n">
         <v>3</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>-10</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="28">
@@ -3408,7 +3534,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1730184635223 - S03 - SANTS - SYNLAB - 16:30</t>
+          <t>1732000704516 - 04 - SANTS - TARDE - W - 15:30</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3417,310 +3543,397 @@
         </is>
       </c>
       <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Sants</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>46</v>
+      </c>
+      <c r="M28" t="n">
+        <v>74</v>
+      </c>
+      <c r="N28" t="n">
+        <v>4</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P28" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1731998639325 - S03 - SANTS - SYNLAB - 16:30</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TRIKE</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>24</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>29/10/2024</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Sants</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>16:24</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>18:31</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>18:41</t>
-        </is>
-      </c>
-      <c r="L28" t="n">
-        <v>85</v>
-      </c>
-      <c r="M28" t="n">
-        <v>127</v>
-      </c>
-      <c r="N28" t="n">
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>125</v>
+      </c>
+      <c r="M29" t="n">
+        <v>167</v>
+      </c>
+      <c r="N29" t="n">
         <v>6</v>
       </c>
-      <c r="O28" t="inlineStr">
+      <c r="O29" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="P28" t="n">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="29"/>
+      <c r="P29" t="n">
+        <v>14</v>
+      </c>
+    </row>
     <row r="30"/>
     <row r="31"/>
     <row r="32"/>
-    <row r="33">
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="C33" s="1" t="inlineStr">
+    <row r="33"/>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D33" s="1" t="inlineStr">
+      <c r="D34" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E33" s="1" t="inlineStr">
+      <c r="E34" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F33" s="1" t="inlineStr">
+      <c r="F34" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="J33" s="1" t="inlineStr">
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J34" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K33" s="1" t="inlineStr">
+      <c r="K34" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L33" s="1" t="inlineStr">
+      <c r="L34" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M33" s="1" t="inlineStr">
+      <c r="M34" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="Q33" s="1" t="inlineStr">
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
+      <c r="Q34" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="R33" s="1" t="inlineStr">
+      <c r="R34" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="S33" s="1" t="inlineStr">
+      <c r="S34" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="T33" s="1" t="inlineStr">
+      <c r="T34" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="B34" s="1" t="n">
+    <row r="35">
+      <c r="B35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>1730184739357</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>10:10</t>
-        </is>
-      </c>
-      <c r="I34" s="1" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1732000314215</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>1730184488854</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>1732000504888</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>09:50</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>11:48</t>
-        </is>
-      </c>
-      <c r="P34" s="1" t="n">
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>12:23</t>
+        </is>
+      </c>
+      <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>1730184819693</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>1731998556866</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
         <is>
           <t>09:50</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>11:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="35"/>
-    <row r="36"/>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>12:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="I36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>1731998598378</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>14:23</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>12</v>
+      </c>
+    </row>
     <row r="37"/>
     <row r="38"/>
     <row r="39"/>
     <row r="40"/>
     <row r="41"/>
-    <row r="42">
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="C42" s="1" t="inlineStr">
+    <row r="42"/>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D42" s="1" t="inlineStr">
+      <c r="D43" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E42" s="1" t="inlineStr">
+      <c r="E43" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F42" s="1" t="inlineStr">
+      <c r="F43" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="J42" s="1" t="inlineStr">
+      <c r="J43" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K42" s="1" t="inlineStr">
+      <c r="K43" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L42" s="1" t="inlineStr">
+      <c r="L43" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M42" s="1" t="inlineStr">
+      <c r="M43" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="B43" s="1" t="n">
+    <row r="44">
+      <c r="B44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1730184584024</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>12:50</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>14:17</t>
-        </is>
-      </c>
-      <c r="I43" s="1" t="n">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1732000594042</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>10:20</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>12:57</t>
+        </is>
+      </c>
+      <c r="I44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>1730185133340</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>1732000704516</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>15:20</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>16:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="I44" s="1" t="n">
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="I45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>1730184635223</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>16:24</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>18:31</t>
-        </is>
-      </c>
-      <c r="M44" t="n">
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1731998639325</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>16:44</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parche 2.1: Arreglat calcul del temps de ruta i aumentat l'espai a excel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -571,19 +571,19 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>10:47</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="L3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M3" t="n">
         <v>84</v>
-      </c>
-      <c r="M3" t="n">
-        <v>147</v>
       </c>
       <c r="N3" t="n">
         <v>9</v>
@@ -631,35 +631,35 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>12:11</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="L4" t="n">
+        <v>29</v>
+      </c>
+      <c r="M4" t="n">
         <v>85</v>
-      </c>
-      <c r="M4" t="n">
-        <v>141</v>
       </c>
       <c r="N4" t="n">
         <v>8</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P4" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="5">
@@ -701,26 +701,26 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>11:55</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>13:29</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="L5" t="n">
+        <v>41</v>
+      </c>
+      <c r="M5" t="n">
         <v>125</v>
-      </c>
-      <c r="M5" t="n">
-        <v>209</v>
       </c>
       <c r="N5" t="n">
         <v>12</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -766,26 +766,26 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:50</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="L6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M6" t="n">
         <v>120</v>
-      </c>
-      <c r="M6" t="n">
-        <v>190</v>
       </c>
       <c r="N6" t="n">
         <v>10</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -826,35 +826,35 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>12:26</t>
         </is>
       </c>
       <c r="L7" t="n">
+        <v>23</v>
+      </c>
+      <c r="M7" t="n">
         <v>86</v>
-      </c>
-      <c r="M7" t="n">
-        <v>149</v>
       </c>
       <c r="N7" t="n">
         <v>9</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>J</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>-3</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="8">
@@ -896,19 +896,19 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>12:51</t>
         </is>
       </c>
       <c r="L8" t="n">
+        <v>34</v>
+      </c>
+      <c r="M8" t="n">
         <v>111</v>
-      </c>
-      <c r="M8" t="n">
-        <v>188</v>
       </c>
       <c r="N8" t="n">
         <v>11</v>
@@ -961,19 +961,19 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>12:44</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>12:54</t>
         </is>
       </c>
       <c r="L9" t="n">
+        <v>30</v>
+      </c>
+      <c r="M9" t="n">
         <v>114</v>
-      </c>
-      <c r="M9" t="n">
-        <v>198</v>
       </c>
       <c r="N9" t="n">
         <v>12</v>
@@ -1026,19 +1026,19 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>18:07</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="L10" t="n">
+        <v>41</v>
+      </c>
+      <c r="M10" t="n">
         <v>104</v>
-      </c>
-      <c r="M10" t="n">
-        <v>167</v>
       </c>
       <c r="N10" t="n">
         <v>9</v>
@@ -1091,26 +1091,26 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>10:37</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>11:36</t>
+          <t>10:47</t>
         </is>
       </c>
       <c r="L11" t="n">
+        <v>28</v>
+      </c>
+      <c r="M11" t="n">
         <v>77</v>
-      </c>
-      <c r="M11" t="n">
-        <v>126</v>
       </c>
       <c r="N11" t="n">
         <v>7</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>M</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -1156,26 +1156,26 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>11:17</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>12:23</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="L12" t="n">
+        <v>31</v>
+      </c>
+      <c r="M12" t="n">
         <v>87</v>
-      </c>
-      <c r="M12" t="n">
-        <v>143</v>
       </c>
       <c r="N12" t="n">
         <v>8</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>K</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -1221,26 +1221,26 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>12:19</t>
+          <t>11:44</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="L13" t="n">
+        <v>79</v>
+      </c>
+      <c r="M13" t="n">
         <v>114</v>
-      </c>
-      <c r="M13" t="n">
-        <v>149</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>F</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1286,19 +1286,19 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>12:57</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="L14" t="n">
+        <v>31</v>
+      </c>
+      <c r="M14" t="n">
         <v>94</v>
-      </c>
-      <c r="M14" t="n">
-        <v>157</v>
       </c>
       <c r="N14" t="n">
         <v>9</v>
@@ -1346,35 +1346,35 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>14:23</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="L15" t="n">
+        <v>66</v>
+      </c>
+      <c r="M15" t="n">
         <v>87</v>
-      </c>
-      <c r="M15" t="n">
-        <v>108</v>
       </c>
       <c r="N15" t="n">
         <v>3</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>-25</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="16">
@@ -1416,26 +1416,26 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>16:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="L16" t="n">
+        <v>18</v>
+      </c>
+      <c r="M16" t="n">
         <v>46</v>
-      </c>
-      <c r="M16" t="n">
-        <v>74</v>
       </c>
       <c r="N16" t="n">
         <v>4</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P16" t="n">
@@ -1476,35 +1476,35 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>16:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="L17" t="n">
+        <v>83</v>
+      </c>
+      <c r="M17" t="n">
         <v>125</v>
-      </c>
-      <c r="M17" t="n">
-        <v>167</v>
       </c>
       <c r="N17" t="n">
         <v>6</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>14</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="18"/>
@@ -1598,11 +1598,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>11:24</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>5.4</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1626,11 +1626,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="5">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1654,11 +1654,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>13:05</t>
+          <t>11:55</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3.5</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="6">
@@ -1672,21 +1672,21 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>09:38</t>
+          <t>10:38</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2.6</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="7">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1710,11 +1710,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>14:13</t>
+          <t>12:46</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3.6</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="8">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>J</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>14:03</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="9">
@@ -1766,114 +1766,114 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>18:12</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>3.1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10"/>
     <row r="11"/>
-    <row r="12">
-      <c r="E12" t="inlineStr">
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="F12">
-        <f>SUM(G3:G9)</f>
+      <c r="F17">
+        <f>SUM(G3:G14)</f>
         <v/>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="L12">
-        <f>SUM(L3:L11)</f>
+      <c r="L17">
+        <f>SUM(L3:L16)</f>
         <v/>
       </c>
     </row>
-    <row r="13">
-      <c r="E13" t="inlineStr">
+    <row r="18">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Num treballadors</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F18" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="E14" t="inlineStr">
+    <row r="19">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Num Rutes</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="F19" t="n">
         <v>8</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>TRIKES</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J19" t="n">
         <v>7</v>
       </c>
-      <c r="K14" s="2">
-        <f>J14/F14</f>
+      <c r="K19" s="2">
+        <f>J19/F19</f>
         <v/>
       </c>
     </row>
-    <row r="15">
-      <c r="E15" t="inlineStr">
+    <row r="20">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Total Paquets</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="F20" t="n">
         <v>80</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>4W</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J20" t="n">
         <v>1</v>
       </c>
-      <c r="K15" s="2">
-        <f>J15/F14</f>
+      <c r="K20" s="2">
+        <f>J20/F19</f>
         <v/>
       </c>
     </row>
-    <row r="16">
-      <c r="I16" t="inlineStr">
+    <row r="21">
+      <c r="I21" t="inlineStr">
         <is>
           <t>TRIKES Min</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="J21" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="17">
-      <c r="I17" t="inlineStr">
+    <row r="22">
+      <c r="I22" t="inlineStr">
         <is>
           <t>4w  Min</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="J22" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
     <row r="23"/>
     <row r="24">
       <c r="C24" s="1" t="inlineStr">
@@ -1986,19 +1986,19 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>10:47</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="L25" t="n">
+        <v>21</v>
+      </c>
+      <c r="M25" t="n">
         <v>84</v>
-      </c>
-      <c r="M25" t="n">
-        <v>147</v>
       </c>
       <c r="N25" t="n">
         <v>9</v>
@@ -2046,35 +2046,35 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>12:11</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="L26" t="n">
+        <v>29</v>
+      </c>
+      <c r="M26" t="n">
         <v>85</v>
-      </c>
-      <c r="M26" t="n">
-        <v>141</v>
       </c>
       <c r="N26" t="n">
         <v>8</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P26" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="27">
@@ -2116,26 +2116,26 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>11:55</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>13:29</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="L27" t="n">
+        <v>41</v>
+      </c>
+      <c r="M27" t="n">
         <v>125</v>
-      </c>
-      <c r="M27" t="n">
-        <v>209</v>
       </c>
       <c r="N27" t="n">
         <v>12</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -2181,26 +2181,26 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:50</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="L28" t="n">
+        <v>50</v>
+      </c>
+      <c r="M28" t="n">
         <v>120</v>
-      </c>
-      <c r="M28" t="n">
-        <v>190</v>
       </c>
       <c r="N28" t="n">
         <v>10</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -2241,35 +2241,35 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>12:26</t>
         </is>
       </c>
       <c r="L29" t="n">
+        <v>23</v>
+      </c>
+      <c r="M29" t="n">
         <v>86</v>
-      </c>
-      <c r="M29" t="n">
-        <v>149</v>
       </c>
       <c r="N29" t="n">
         <v>9</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>J</t>
         </is>
       </c>
       <c r="P29" t="n">
-        <v>-3</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="30">
@@ -2311,19 +2311,19 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>12:51</t>
         </is>
       </c>
       <c r="L30" t="n">
+        <v>34</v>
+      </c>
+      <c r="M30" t="n">
         <v>111</v>
-      </c>
-      <c r="M30" t="n">
-        <v>188</v>
       </c>
       <c r="N30" t="n">
         <v>11</v>
@@ -2376,19 +2376,19 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>12:44</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>12:54</t>
         </is>
       </c>
       <c r="L31" t="n">
+        <v>30</v>
+      </c>
+      <c r="M31" t="n">
         <v>114</v>
-      </c>
-      <c r="M31" t="n">
-        <v>198</v>
       </c>
       <c r="N31" t="n">
         <v>12</v>
@@ -2441,19 +2441,19 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>18:07</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="L32" t="n">
+        <v>41</v>
+      </c>
+      <c r="M32" t="n">
         <v>104</v>
-      </c>
-      <c r="M32" t="n">
-        <v>167</v>
       </c>
       <c r="N32" t="n">
         <v>9</v>
@@ -2499,32 +2499,32 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J37" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="K37" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="L37" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="M37" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
           <t>D</t>
-        </is>
-      </c>
-      <c r="J37" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="K37" s="1" t="inlineStr">
-        <is>
-          <t>Inici Ruta</t>
-        </is>
-      </c>
-      <c r="L37" s="1" t="inlineStr">
-        <is>
-          <t>Fi Ruta</t>
-        </is>
-      </c>
-      <c r="M37" s="1" t="inlineStr">
-        <is>
-          <t>Temps Espera Min</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>F</t>
         </is>
       </c>
       <c r="Q37" s="1" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="I38" s="1" t="n">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>11:55</t>
         </is>
       </c>
       <c r="P38" s="1" t="n">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:50</t>
         </is>
       </c>
     </row>
@@ -2610,17 +2610,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1731999265927</t>
+          <t>1731999790486</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -2636,7 +2636,7 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>G</t>
         </is>
       </c>
       <c r="J46" s="1" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>J</t>
         </is>
       </c>
       <c r="Q46" s="1" t="inlineStr">
@@ -2716,17 +2716,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1731999790486</t>
+          <t>1731999561009</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>12:11</t>
+          <t>12:44</t>
         </is>
       </c>
       <c r="I47" s="1" t="n">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>1731999561009</t>
+          <t>1731999825299</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="P47" s="1" t="n">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>1731999825299</t>
+          <t>1731999265927</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>12:16</t>
         </is>
       </c>
     </row>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>18:07</t>
+          <t>17:04</t>
         </is>
       </c>
     </row>
@@ -2831,7 +2831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2910,11 +2910,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="4">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>14:28</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>4.8</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="5">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2966,11 +2966,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>11:22</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="6">
@@ -2994,11 +2994,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="7">
@@ -3012,269 +3012,232 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>14:22</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sants</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>15:08</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>19:36</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="8"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>18:26</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
     <row r="9"/>
-    <row r="10">
-      <c r="E10" t="inlineStr">
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="F10">
-        <f>SUM(G3:G7)</f>
+      <c r="F16">
+        <f>SUM(G3:G13)</f>
         <v/>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Total Hores</t>
         </is>
       </c>
-      <c r="L10">
-        <f>SUM(L3:L9)</f>
+      <c r="L16">
+        <f>SUM(L3:L15)</f>
         <v/>
       </c>
     </row>
-    <row r="11">
-      <c r="E11" t="inlineStr">
+    <row r="17">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Num treballadors</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="E12" t="inlineStr">
+      <c r="F17" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Num Rutes</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="F18" t="n">
         <v>7</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>TRIKES</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="J18" t="n">
         <v>7</v>
       </c>
-      <c r="K12" s="2">
-        <f>J12/F12</f>
+      <c r="K18" s="2">
+        <f>J18/F18</f>
         <v/>
       </c>
     </row>
-    <row r="13">
-      <c r="E13" t="inlineStr">
+    <row r="19">
+      <c r="E19" t="inlineStr">
         <is>
           <t>Total Paquets</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F19" t="n">
         <v>42</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>4W</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J19" t="n">
         <v>0</v>
       </c>
-      <c r="K13" s="2">
-        <f>J13/F12</f>
+      <c r="K19" s="2">
+        <f>J19/F18</f>
         <v/>
       </c>
     </row>
-    <row r="14">
-      <c r="I14" t="inlineStr">
+    <row r="20">
+      <c r="I20" t="inlineStr">
         <is>
           <t>TRIKES Min</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J20" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="15">
-      <c r="I15" t="inlineStr">
+    <row r="21">
+      <c r="I21" t="inlineStr">
         <is>
           <t>4w  Min</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J21" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22">
-      <c r="C22" s="1" t="inlineStr">
+    <row r="22"/>
+    <row r="23">
+      <c r="C23" s="1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="D22" s="1" t="inlineStr">
+      <c r="D23" s="1" t="inlineStr">
         <is>
           <t>Tipus Bici</t>
         </is>
       </c>
-      <c r="E22" s="1" t="inlineStr">
+      <c r="E23" s="1" t="inlineStr">
         <is>
           <t>Pes</t>
         </is>
       </c>
-      <c r="F22" s="1" t="inlineStr">
+      <c r="F23" s="1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="G22" s="1" t="inlineStr">
+      <c r="G23" s="1" t="inlineStr">
         <is>
           <t>Hub</t>
         </is>
       </c>
-      <c r="H22" s="1" t="inlineStr">
+      <c r="H23" s="1" t="inlineStr">
         <is>
           <t>Hora Inici Ruta Plnif</t>
         </is>
       </c>
-      <c r="I22" s="1" t="inlineStr">
+      <c r="I23" s="1" t="inlineStr">
         <is>
           <t>Hora Inici Ruta Real</t>
         </is>
       </c>
-      <c r="J22" s="1" t="inlineStr">
+      <c r="J23" s="1" t="inlineStr">
         <is>
           <t>Hora Fi Ruta</t>
         </is>
       </c>
-      <c r="K22" s="1" t="inlineStr">
+      <c r="K23" s="1" t="inlineStr">
         <is>
           <t>Inici Seguent Ruta</t>
         </is>
       </c>
-      <c r="L22" s="1" t="inlineStr">
+      <c r="L23" s="1" t="inlineStr">
         <is>
           <t>Temps Recorregut Ruta</t>
         </is>
       </c>
-      <c r="M22" s="1" t="inlineStr">
+      <c r="M23" s="1" t="inlineStr">
         <is>
           <t>Temps Total Ruta</t>
         </is>
       </c>
-      <c r="N22" s="1" t="inlineStr">
+      <c r="N23" s="1" t="inlineStr">
         <is>
           <t>Num Entregues</t>
         </is>
       </c>
-      <c r="O22" s="1" t="inlineStr">
+      <c r="O23" s="1" t="inlineStr">
         <is>
           <t>Assignació</t>
         </is>
       </c>
-      <c r="P22" s="1" t="inlineStr">
+      <c r="P23" s="1" t="inlineStr">
         <is>
           <t>Plnif vs Real Min</t>
         </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>1732000314215 - 01 - SANTS - ESTACIO - W - 09:30</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>TRIKE</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>48</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>19/11/2024</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Sants</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>9:30</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>11:26</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>11:36</t>
-        </is>
-      </c>
-      <c r="L23" t="n">
-        <v>77</v>
-      </c>
-      <c r="M23" t="n">
-        <v>126</v>
-      </c>
-      <c r="N23" t="n">
-        <v>7</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="P23" t="n">
-        <v>-10</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1732000504888 - 02 - SANTS - DIAGONAL - 10:00</t>
+          <t>1732000314215 - 01 - SANTS - ESTACIO - W - 09:30</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -3283,7 +3246,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -3297,36 +3260,36 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>09:50</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>10:37</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>12:23</t>
+          <t>10:47</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="M24" t="n">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="N24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>M</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -3335,11 +3298,11 @@
     </row>
     <row r="25">
       <c r="B25" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1731998556866 - S01 - SANTS - SYNLAB - 10:00</t>
+          <t>1732000504888 - 02 - SANTS - DIAGONAL - 10:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3348,7 +3311,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -3372,26 +3335,26 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>12:19</t>
+          <t>11:17</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>12:29</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="M25" t="n">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="N25" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -3400,11 +3363,11 @@
     </row>
     <row r="26">
       <c r="B26" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1732000594042 - 03 - SANTS - URGELL 10:30</t>
+          <t>1731998556866 - S01 - SANTS - SYNLAB - 10:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -3413,7 +3376,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -3427,36 +3390,36 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>10:20</t>
+          <t>09:50</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>12:57</t>
+          <t>11:44</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="M26" t="n">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="N26" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>F</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -3465,11 +3428,11 @@
     </row>
     <row r="27">
       <c r="B27" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1731998598378 - S02 - SANTS - SYNLAB - 13:00</t>
+          <t>1732000594042 - 03 - SANTS - URGELL 10:30</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -3478,7 +3441,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -3492,49 +3455,49 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>10:20</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>14:23</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="M27" t="n">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="N27" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>I</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>-25</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1732000704516 - 04 - SANTS - TARDE - W - 15:30</t>
+          <t>1731998598378 - S02 - SANTS - SYNLAB - 13:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3543,7 +3506,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -3557,36 +3520,36 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>16:44</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="M28" t="n">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="N28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -3595,227 +3558,269 @@
     </row>
     <row r="29">
       <c r="B29" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1732000704516 - 04 - SANTS - TARDE - W - 15:30</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TRIKE</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Sants</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>16:06</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>18</v>
+      </c>
+      <c r="M29" t="n">
+        <v>46</v>
+      </c>
+      <c r="N29" t="n">
+        <v>4</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P29" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>1731998639325 - S03 - SANTS - SYNLAB - 16:30</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>TRIKE</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="E30" t="n">
         <v>24</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>19/11/2024</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>Sants</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>16:44</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>19:31</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>19:41</t>
-        </is>
-      </c>
-      <c r="L29" t="n">
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>83</v>
+      </c>
+      <c r="M30" t="n">
         <v>125</v>
       </c>
-      <c r="M29" t="n">
-        <v>167</v>
-      </c>
-      <c r="N29" t="n">
+      <c r="N30" t="n">
         <v>6</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P29" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30"/>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P30" t="n">
+        <v>-14</v>
+      </c>
+    </row>
     <row r="31"/>
     <row r="32"/>
     <row r="33"/>
-    <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="C34" s="1" t="inlineStr">
+    <row r="34"/>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D34" s="1" t="inlineStr">
+      <c r="D35" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E34" s="1" t="inlineStr">
+      <c r="E35" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F34" s="1" t="inlineStr">
+      <c r="F35" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="J34" s="1" t="inlineStr">
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="J35" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K34" s="1" t="inlineStr">
+      <c r="K35" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L34" s="1" t="inlineStr">
+      <c r="L35" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M34" s="1" t="inlineStr">
+      <c r="M35" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="Q34" s="1" t="inlineStr">
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="Q35" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="R34" s="1" t="inlineStr">
+      <c r="R35" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="S34" s="1" t="inlineStr">
+      <c r="S35" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="T34" s="1" t="inlineStr">
+      <c r="T35" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="B35" s="1" t="n">
+    <row r="36">
+      <c r="B36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>1732000314215</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>09:20</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>11:26</t>
-        </is>
-      </c>
-      <c r="I35" s="1" t="n">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>10:37</t>
+        </is>
+      </c>
+      <c r="I36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>1731998556866</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>11:44</t>
+        </is>
+      </c>
+      <c r="P36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="inlineStr">
         <is>
           <t>1732000504888</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="R36" t="inlineStr">
         <is>
           <t>09:50</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>12:23</t>
-        </is>
-      </c>
-      <c r="P35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>1731998556866</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>09:50</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>12:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="I36" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>1731998598378</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>12:35</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>14:23</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>12</v>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>11:17</t>
+        </is>
       </c>
     </row>
     <row r="37"/>
@@ -3824,116 +3829,160 @@
     <row r="40"/>
     <row r="41"/>
     <row r="42"/>
-    <row r="43">
-      <c r="B43" t="inlineStr">
+    <row r="43"/>
+    <row r="44">
+      <c r="B44" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="C43" s="1" t="inlineStr">
+      <c r="C44" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D43" s="1" t="inlineStr">
+      <c r="D44" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="E43" s="1" t="inlineStr">
+      <c r="E44" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="F43" s="1" t="inlineStr">
+      <c r="F44" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J43" s="1" t="inlineStr">
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="J44" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="K43" s="1" t="inlineStr">
+      <c r="K44" s="1" t="inlineStr">
         <is>
           <t>Inici Ruta</t>
         </is>
       </c>
-      <c r="L43" s="1" t="inlineStr">
+      <c r="L44" s="1" t="inlineStr">
         <is>
           <t>Fi Ruta</t>
         </is>
       </c>
-      <c r="M43" s="1" t="inlineStr">
+      <c r="M44" s="1" t="inlineStr">
         <is>
           <t>Temps Espera Min</t>
         </is>
       </c>
-    </row>
-    <row r="44">
-      <c r="B44" s="1" t="n">
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Q44" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="R44" s="1" t="inlineStr">
+        <is>
+          <t>Inici Ruta</t>
+        </is>
+      </c>
+      <c r="S44" s="1" t="inlineStr">
+        <is>
+          <t>Fi Ruta</t>
+        </is>
+      </c>
+      <c r="T44" s="1" t="inlineStr">
+        <is>
+          <t>Temps Espera Min</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>1732000594042</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>10:20</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>12:57</t>
-        </is>
-      </c>
-      <c r="I44" s="1" t="n">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="I45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1731998598378</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="inlineStr">
         <is>
           <t>1732000704516</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="R45" t="inlineStr">
         <is>
           <t>15:20</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>16:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="I45" s="1" t="n">
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="P46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="Q46" t="inlineStr">
         <is>
           <t>1731998639325</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>16:44</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>19:31</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="T46" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>